<commit_message>
add resource(), edit resource(), delete resource() added
</commit_message>
<xml_diff>
--- a/resources/TestDataForResourceAddingToDB.xlsx
+++ b/resources/TestDataForResourceAddingToDB.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
-    <t>Новий ресурс для DAO у верхньому меню</t>
-  </si>
-  <si>
     <t>Контент нового ресурсу для DAO</t>
   </si>
   <si>
@@ -30,9 +27,6 @@
     <t>AliasForDAO2</t>
   </si>
   <si>
-    <t>Новий ресурс для DAO в розділі "Ресурси"</t>
-  </si>
-  <si>
     <t>alias</t>
   </si>
   <si>
@@ -54,9 +48,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>Ресурс відредактований</t>
-  </si>
-  <si>
     <t>Контект відредактований</t>
   </si>
   <si>
@@ -64,6 +55,15 @@
   </si>
   <si>
     <t>addTextToContent</t>
+  </si>
+  <si>
+    <t>відредагований</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Новий ресурс вверху </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Новий ресурс в меню </t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,25 +423,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -449,22 +449,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -472,22 +472,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>